<commit_message>
Finished BUSE 120 module 4 notes
</commit_message>
<xml_diff>
--- a/school/files/fall-2020/BUSE-120/module-3/financial_worksheets_module-3.xlsx
+++ b/school/files/fall-2020/BUSE-120/module-3/financial_worksheets_module-3.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8694C964-887D-49DA-8641-01A35B370E11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C16DBA-77DB-42D0-9AE7-C4C577ADE259}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16530" yWindow="0" windowWidth="21870" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Balance Sheet" sheetId="5" r:id="rId1"/>
@@ -340,9 +340,6 @@
     <t>TOTAL LONG-TERM LIABILITIES</t>
   </si>
   <si>
-    <t>Vehicle loan</t>
-  </si>
-  <si>
     <t>Home mortgage</t>
   </si>
   <si>
@@ -428,6 +425,9 @@
   </si>
   <si>
     <t>Car Insurance</t>
+  </si>
+  <si>
+    <t>Vehicle loan (lease)</t>
   </si>
 </sst>
 </file>
@@ -1366,7 +1366,7 @@
     <dxf>
       <font>
         <b/>
-        <i/>
+        <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
@@ -1380,14 +1380,14 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0"/>
+      <numFmt numFmtId="10" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -1430,62 +1430,8 @@
       <font>
         <b/>
         <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
+        <color rgb="FFFF0000"/>
       </font>
-      <numFmt numFmtId="10" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -1520,6 +1466,9 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="9" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1550,6 +1499,17 @@
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="9" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1584,36 +1544,15 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="9" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
+      <numFmt numFmtId="165" formatCode="_)@"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="2"/>
+          <bgColor theme="0"/>
         </patternFill>
       </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1648,6 +1587,52 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="9" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="9" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="9" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1678,6 +1663,138 @@
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_)@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="9" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="9" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="9" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="9" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="_)@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.89999084444715716"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_)@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1727,6 +1844,31 @@
         <sz val="10"/>
         <color auto="1"/>
         <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="13" formatCode="0%"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
@@ -1744,6 +1886,15 @@
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="9" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1778,6 +1929,17 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="9" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1808,76 +1970,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="9" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="9" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_)@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="13" formatCode="0%"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="9" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="9" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="_)@"/>
@@ -1923,6 +2015,9 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="9" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1953,6 +2048,16 @@
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="9" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1987,138 +2092,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="9" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="9" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="_)@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.89999084444715716"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="10" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="9" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="9" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="165" formatCode="_)@"/>
       <fill>
         <patternFill patternType="solid">
@@ -2130,121 +2103,9 @@
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="9" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="9" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_)@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="9" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="9" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_)@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="10" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0"/>
       <alignment horizontal="left" vertical="center" textRotation="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0"/>
@@ -2356,9 +2217,72 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0"/>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0"/>
@@ -2392,6 +2316,82 @@
     <dxf>
       <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0"/>
       <alignment horizontal="left" vertical="center" textRotation="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="10" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="10" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -5806,8 +5806,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="30" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="tblCurrentAssets" displayName="tblCurrentAssets" ref="B9:C25" totalsRowCount="1" headerRowDxfId="56" dataDxfId="55" totalsRowDxfId="54">
   <autoFilter ref="B9:C24" xr:uid="{00000000-0009-0000-0100-00001E000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="FINANCIAL ASSETS" totalsRowLabel="TOTAL FINANCIAL ASSETS" dataDxfId="28" totalsRowDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="VALUE" totalsRowFunction="sum" dataDxfId="27" totalsRowDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="FINANCIAL ASSETS" totalsRowLabel="TOTAL FINANCIAL ASSETS" dataDxfId="53" totalsRowDxfId="52"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="VALUE" totalsRowFunction="sum" dataDxfId="51" totalsRowDxfId="50"/>
   </tableColumns>
   <tableStyleInfo name="Balance sheet table" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -5819,11 +5819,11 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="31" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="tblOtherAssets" displayName="tblOtherAssets" ref="B27:C40" totalsRowCount="1" dataDxfId="53" totalsRowDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="31" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="tblOtherAssets" displayName="tblOtherAssets" ref="B27:C40" totalsRowCount="1" dataDxfId="49" totalsRowDxfId="48">
   <autoFilter ref="B27:C39" xr:uid="{00000000-0009-0000-0100-00001F000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="TANGIBLE ASSETS" totalsRowLabel="TOTAL TANGIBLE ASSETS" dataDxfId="51" totalsRowDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="VALUE" totalsRowFunction="sum" dataDxfId="50" totalsRowDxfId="0" dataCellStyle="Currency" totalsRowCellStyle="Currency"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="TANGIBLE ASSETS" totalsRowLabel="TOTAL TANGIBLE ASSETS" dataDxfId="47" totalsRowDxfId="46"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="VALUE" totalsRowFunction="sum" dataDxfId="45" totalsRowDxfId="44" dataCellStyle="Currency" totalsRowCellStyle="Currency"/>
   </tableColumns>
   <tableStyleInfo name="Balance sheet table" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -5835,11 +5835,11 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="32" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="tblCurrentLiabilities" displayName="tblCurrentLiabilities" ref="E9:F19" totalsRowCount="1" headerRowDxfId="49" dataDxfId="48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="32" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="tblCurrentLiabilities" displayName="tblCurrentLiabilities" ref="E9:F19" totalsRowCount="1" headerRowDxfId="43" dataDxfId="42">
   <autoFilter ref="E9:F18" xr:uid="{00000000-0009-0000-0100-000020000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="SHORT-TERM LIABILITIES" totalsRowLabel="TOTAL SHORT-TERM LIABILITIES" dataDxfId="47" totalsRowDxfId="46"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="AMOUNT" totalsRowFunction="sum" dataDxfId="45" totalsRowDxfId="44"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="SHORT-TERM LIABILITIES" totalsRowLabel="TOTAL SHORT-TERM LIABILITIES" dataDxfId="41" totalsRowDxfId="40"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="AMOUNT" totalsRowFunction="sum" dataDxfId="39" totalsRowDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="Balance sheet table" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -5851,11 +5851,11 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="33" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="tblOtherLiabilities" displayName="tblOtherLiabilities" ref="E21:F30" totalsRowCount="1" dataDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="33" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="tblOtherLiabilities" displayName="tblOtherLiabilities" ref="E21:F30" totalsRowCount="1" dataDxfId="37">
   <autoFilter ref="E21:F29" xr:uid="{00000000-0009-0000-0100-000021000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="LONG-TERM LIABILITIES" totalsRowLabel="TOTAL LONG-TERM LIABILITIES" dataDxfId="42" totalsRowDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="AMOUNT" totalsRowFunction="sum" dataDxfId="40" totalsRowDxfId="39"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="LONG-TERM LIABILITIES" totalsRowLabel="TOTAL LONG-TERM LIABILITIES" dataDxfId="36" totalsRowDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="AMOUNT" totalsRowFunction="sum" dataDxfId="35" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Balance sheet table" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -5869,9 +5869,9 @@
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="tblIncome" displayName="tblIncome" ref="B30:D37" totalsRowCount="1">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Total Income" totalsRowLabel="  Total" dataDxfId="38" totalsRowDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Annual  " totalsRowFunction="sum" dataDxfId="37" totalsRowDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Monthly " totalsRowFunction="sum" dataDxfId="36" totalsRowDxfId="24">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Total Income" totalsRowLabel="  Total" dataDxfId="34" totalsRowDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Annual  " totalsRowFunction="sum" dataDxfId="32" totalsRowDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Monthly " totalsRowFunction="sum" dataDxfId="30" totalsRowDxfId="29">
       <calculatedColumnFormula>tblIncome[[#This Row],[Annual  ]]/12</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5882,15 +5882,15 @@
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="tblExpenses" displayName="tblExpenses" ref="G30:J51" totalsRowCount="1">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Living Expenses" totalsRowLabel=" Total" dataDxfId="20" totalsRowDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Annual  " totalsRowFunction="custom" dataDxfId="19" totalsRowDxfId="12">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Living Expenses" totalsRowLabel=" Total" dataDxfId="28" totalsRowDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Annual  " totalsRowFunction="custom" dataDxfId="26" totalsRowDxfId="25">
       <totalsRowFormula>SUM(tblExpenses[[Annual  ]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Monthly " totalsRowFunction="custom" dataDxfId="18" totalsRowDxfId="11">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Monthly " totalsRowFunction="custom" dataDxfId="24" totalsRowDxfId="23">
       <calculatedColumnFormula>tblExpenses[[#This Row],[Annual  ]]/12</calculatedColumnFormula>
       <totalsRowFormula>SUM(tblExpenses[[Monthly ]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="% Income" totalsRowFunction="custom" dataDxfId="17" totalsRowDxfId="10">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="% Income" totalsRowFunction="custom" dataDxfId="22" totalsRowDxfId="21">
       <calculatedColumnFormula>IF($D$37=0,"",I31/$D$37)</calculatedColumnFormula>
       <totalsRowFormula>IF($D$37=0,"",I51/$D$37)</totalsRowFormula>
     </tableColumn>
@@ -5902,9 +5902,9 @@
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="tblDiscretionary" displayName="tblDiscretionary" ref="L30:N45" totalsRowCount="1">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Discretionary Expenses" totalsRowLabel="  Total" dataDxfId="16" totalsRowDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Annual  " totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="Monthly " totalsRowFunction="sum" dataDxfId="14" totalsRowDxfId="7">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Discretionary Expenses" totalsRowLabel="  Total" dataDxfId="20" totalsRowDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Annual  " totalsRowFunction="sum" dataDxfId="18" totalsRowDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="Monthly " totalsRowFunction="sum" dataDxfId="16" totalsRowDxfId="15">
       <calculatedColumnFormula>tblDiscretionary[[#This Row],[Annual  ]]/12</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5915,9 +5915,9 @@
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="tblSavings" displayName="tblSavings" ref="Q30:S36" totalsRowCount="1">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Savings/Investments" totalsRowLabel="Total" dataDxfId="35" totalsRowDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Annual  " totalsRowFunction="sum" dataDxfId="34" totalsRowDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Monthly " totalsRowFunction="sum" dataDxfId="33" totalsRowDxfId="4">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Savings/Investments" totalsRowLabel="Total" dataDxfId="14" totalsRowDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Annual  " totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Monthly " totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="9">
       <calculatedColumnFormula>tblSavings[[#This Row],[Annual  ]]/12</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5928,9 +5928,9 @@
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="39" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="tblIncome40" displayName="tblIncome40" ref="B39:D46" totalsRowCount="1">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Income Withholdings" totalsRowLabel=" Total " dataDxfId="32" totalsRowDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="Annual  " totalsRowFunction="sum" dataDxfId="31" totalsRowDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="Monthly " totalsRowFunction="sum" dataDxfId="30" totalsRowDxfId="21">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Income Withholdings" totalsRowLabel=" Total " dataDxfId="8" totalsRowDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="Annual  " totalsRowFunction="sum" dataDxfId="6" totalsRowDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="Monthly " totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="3">
       <calculatedColumnFormula>tblIncome40[[#This Row],[Annual  ]]/12</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -6170,8 +6170,8 @@
   </sheetPr>
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6198,7 +6198,7 @@
     <row r="2" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2"/>
       <c r="B2" s="138" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C2" s="26"/>
       <c r="D2" s="26"/>
@@ -6268,14 +6268,14 @@
         <v>59</v>
       </c>
       <c r="C9" s="49" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D9" s="24"/>
       <c r="E9" s="48" t="s">
         <v>57</v>
       </c>
       <c r="F9" s="50" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -6287,7 +6287,7 @@
       </c>
       <c r="D10" s="19"/>
       <c r="E10" s="136" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F10" s="137">
         <v>0</v>
@@ -6325,7 +6325,7 @@
     </row>
     <row r="13" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B13" s="134" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C13" s="135">
         <v>0</v>
@@ -6340,7 +6340,7 @@
     </row>
     <row r="14" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B14" s="134" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C14" s="135">
         <v>0</v>
@@ -6383,7 +6383,7 @@
     </row>
     <row r="17" spans="2:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B17" s="134" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C17" s="135">
         <v>0</v>
@@ -6409,7 +6409,7 @@
     </row>
     <row r="19" spans="2:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B19" s="134" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C19" s="135">
         <v>0</v>
@@ -6425,7 +6425,7 @@
     </row>
     <row r="20" spans="2:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B20" s="134" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C20" s="135">
         <v>0</v>
@@ -6444,7 +6444,7 @@
         <v>58</v>
       </c>
       <c r="F21" s="50" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="2:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -6454,7 +6454,7 @@
       <c r="C22" s="135"/>
       <c r="D22" s="19"/>
       <c r="E22" s="136" t="s">
-        <v>102</v>
+        <v>131</v>
       </c>
       <c r="F22" s="137">
         <v>5739</v>
@@ -6467,7 +6467,7 @@
       <c r="C23" s="135"/>
       <c r="D23" s="19"/>
       <c r="E23" s="136" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F23" s="137">
         <v>0</v>
@@ -6512,7 +6512,7 @@
         <v>60</v>
       </c>
       <c r="C27" s="50" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E27" s="136" t="s">
         <v>48</v>
@@ -6571,7 +6571,7 @@
     </row>
     <row r="32" spans="2:6" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B32" s="136" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C32" s="137">
         <v>2000</v>
@@ -6594,7 +6594,7 @@
     </row>
     <row r="34" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="136" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C34" s="137">
         <v>600</v>
@@ -6661,7 +6661,7 @@
     <row r="43" spans="2:6" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="44" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="146" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -6691,7 +6691,7 @@
   </sheetPr>
   <dimension ref="A1:AJ61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A6" workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
@@ -6715,7 +6715,7 @@
     <row r="1" spans="1:36" s="1" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1"/>
       <c r="B1" s="33" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H1" s="28"/>
       <c r="I1" s="28"/>
@@ -6750,7 +6750,7 @@
     <row r="2" spans="1:36" s="16" customFormat="1" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A2"/>
       <c r="B2" s="138" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C2" s="27"/>
       <c r="D2" s="27"/>
@@ -6847,7 +6847,7 @@
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
       <c r="Q6" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="R6" s="2"/>
       <c r="S6" s="2"/>
@@ -7299,7 +7299,7 @@
     </row>
     <row r="30" spans="2:20" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B30" s="58" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>27</v>
@@ -7308,7 +7308,7 @@
         <v>26</v>
       </c>
       <c r="E30" s="68" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G30" s="58" t="s">
         <v>29</v>
@@ -7320,7 +7320,7 @@
         <v>26</v>
       </c>
       <c r="J30" s="68" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L30" s="58" t="s">
         <v>9</v>
@@ -7332,10 +7332,10 @@
         <v>26</v>
       </c>
       <c r="O30" s="68" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="Q30" s="58" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="R30" s="7" t="s">
         <v>27</v>
@@ -7344,7 +7344,7 @@
         <v>26</v>
       </c>
       <c r="T30" s="68" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="2:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -7514,7 +7514,7 @@
       </c>
       <c r="P33" s="36"/>
       <c r="Q33" s="56" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="R33" s="57">
         <v>1440</v>
@@ -7573,7 +7573,7 @@
       </c>
       <c r="P34" s="36"/>
       <c r="Q34" s="56" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="R34" s="57">
         <v>600</v>
@@ -7659,7 +7659,7 @@
       </c>
       <c r="F36" s="36"/>
       <c r="G36" s="56" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H36" s="57">
         <v>0</v>
@@ -7801,7 +7801,7 @@
         <v>1</v>
       </c>
       <c r="T38" s="68" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="39" spans="2:20" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7815,7 +7815,7 @@
         <v>26</v>
       </c>
       <c r="E39" s="68" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F39" s="36"/>
       <c r="G39" s="56" t="s">
@@ -7909,7 +7909,7 @@
       </c>
       <c r="P40" s="36"/>
       <c r="Q40" s="61" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="R40" s="41">
         <f>R36</f>
@@ -7941,7 +7941,7 @@
       </c>
       <c r="F41" s="36"/>
       <c r="G41" s="56" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H41" s="57">
         <v>1440</v>
@@ -8239,7 +8239,7 @@
         <v>1</v>
       </c>
       <c r="O47" s="68" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="P47" s="36"/>
       <c r="Q47" s="36"/>
@@ -8258,7 +8258,7 @@
         <v>1</v>
       </c>
       <c r="E48" s="68" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F48" s="36"/>
       <c r="G48" s="56" t="s">
@@ -8297,7 +8297,7 @@
     </row>
     <row r="49" spans="2:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="63" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C49" s="64">
         <f>tblIncome[[#Totals],[Annual  ]]</f>
@@ -8504,7 +8504,7 @@
     <row r="1" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1"/>
       <c r="B1" s="33" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C1" s="26"/>
     </row>
@@ -8528,7 +8528,7 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="155" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C5" s="155"/>
     </row>
@@ -8538,25 +8538,25 @@
     </row>
     <row r="7" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="126" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C7" s="139"/>
     </row>
     <row r="8" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="127" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C8" s="140"/>
     </row>
     <row r="9" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="126" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C9" s="141"/>
     </row>
     <row r="10" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="128" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C10" s="129" t="str">
         <f>IF(C9=0,"",(C7*(C8/12)/(((1+(C8/12))^C9)-1)))</f>
@@ -10115,7 +10115,7 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <conditionalFormatting sqref="H6:H62">
-    <cfRule type="cellIs" dxfId="29" priority="1" operator="notBetween">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="notBetween">
       <formula>-0.05</formula>
       <formula>0.05</formula>
     </cfRule>

</xml_diff>